<commit_message>
put all the files together in the main folder of the repository
</commit_message>
<xml_diff>
--- a/SP6T-COTS-System-Build-BOM.xlsx
+++ b/SP6T-COTS-System-Build-BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\MEMSduino\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3547052D-C287-4B24-8CB1-0F8761E55AC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABB6136E-03B9-4EFB-99CF-F4BC01D0EA07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{964DCA75-9C03-4665-A5C3-D212B2818574}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="115">
   <si>
     <t>description</t>
   </si>
@@ -356,13 +356,31 @@
     <t>Momentary buttons</t>
   </si>
   <si>
-    <t>wood board</t>
-  </si>
-  <si>
     <t>https://www.amazon.com/Stainless-Phillips-Screws-Multipurpose-TPOHH/dp/B0CHRWGT8N</t>
   </si>
   <si>
     <t>Ocooch Hardwoods</t>
+  </si>
+  <si>
+    <t>https://ocoochhardwoods.com/detail/?i=124wo</t>
+  </si>
+  <si>
+    <t>1/2" White oak board, 4" x 24"</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/sparkfun-electronics/PRT-12795/5993860</t>
+  </si>
+  <si>
+    <t>1568-1512-ND</t>
+  </si>
+  <si>
+    <t>Sparkfun</t>
+  </si>
+  <si>
+    <t>PRT-12795</t>
+  </si>
+  <si>
+    <t>JUMPER WIRE M/M 6" 20PCS</t>
   </si>
 </sst>
 </file>
@@ -758,10 +776,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9227DDD-8365-4864-A5FB-3571E7A7DE36}">
-  <dimension ref="A1:I38"/>
+  <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -807,740 +825,787 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>109</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>108</v>
       </c>
       <c r="C2" s="2">
-        <v>3.73</v>
+        <v>5.4</v>
       </c>
       <c r="D2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E2" s="2">
-        <f t="shared" ref="E2:E5" si="0">$C2*$D2</f>
-        <v>7.46</v>
+        <f>$C2*$D2</f>
+        <v>5.4</v>
       </c>
       <c r="F2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" t="s">
-        <v>12</v>
+        <v>107</v>
+      </c>
+      <c r="H2" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>13</v>
+        <v>32</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="C3" s="2">
-        <v>1.2</v>
+        <v>1.62</v>
       </c>
       <c r="D3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E3" s="2">
-        <f t="shared" si="0"/>
-        <v>2.4</v>
+        <f>$C3*$D3</f>
+        <v>6.48</v>
       </c>
       <c r="F3" t="s">
         <v>9</v>
       </c>
       <c r="G3" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>80</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>17</v>
+        <v>106</v>
       </c>
       <c r="C4" s="2">
-        <v>0.05</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="D4">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E4" s="2">
-        <f t="shared" si="0"/>
-        <v>0.1</v>
+        <f>$C4*$D4</f>
+        <v>0.56000000000000005</v>
       </c>
       <c r="F4" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="G4" t="s">
-        <v>18</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="2">
-        <v>1.7999999999999999E-2</v>
+        <v>79</v>
       </c>
       <c r="D5">
-        <v>9</v>
-      </c>
-      <c r="E5" s="2">
-        <f t="shared" si="0"/>
-        <v>0.16199999999999998</v>
+        <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" t="s">
-        <v>21</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>80</v>
+        <v>45</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="C6" s="2">
-        <v>7.0000000000000007E-2</v>
+        <v>75</v>
       </c>
       <c r="D6">
-        <v>8</v>
-      </c>
-      <c r="E6" s="2">
-        <f t="shared" ref="E6:E7" si="1">$C6*$D6</f>
-        <v>0.56000000000000005</v>
+        <v>1</v>
       </c>
       <c r="F6" t="s">
-        <v>44</v>
-      </c>
-      <c r="G6" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C7" s="2">
-        <v>1.62</v>
+        <v>75</v>
       </c>
       <c r="D7">
-        <v>4</v>
-      </c>
-      <c r="E7" s="2">
-        <f t="shared" si="1"/>
-        <v>6.48</v>
+        <v>2</v>
       </c>
       <c r="F7" t="s">
-        <v>9</v>
-      </c>
-      <c r="G7" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>106</v>
+        <v>35</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="2">
+        <v>8.1000000000000003E-2</v>
+      </c>
+      <c r="D8">
+        <v>7</v>
+      </c>
+      <c r="E8" s="2">
+        <f>$C8*$D8</f>
+        <v>0.56700000000000006</v>
       </c>
       <c r="F8" t="s">
-        <v>108</v>
+        <v>60</v>
+      </c>
+      <c r="G8" t="s">
+        <v>62</v>
+      </c>
+      <c r="H8" t="s">
+        <v>61</v>
+      </c>
+      <c r="I8" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="C9" s="2">
-        <v>14.9</v>
+        <v>0.47</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E9" s="2">
         <f>$C9*$D9</f>
-        <v>14.9</v>
+        <v>1.88</v>
       </c>
       <c r="F9" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="G9" t="s">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="H9" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="I9" t="s">
-        <v>72</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="C10" s="2">
-        <v>0.1</v>
+        <v>1.7999999999999999E-2</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E10" s="2">
         <f>$C10*$D10</f>
-        <v>0.1</v>
+        <v>0.16199999999999998</v>
       </c>
       <c r="F10" t="s">
-        <v>42</v>
+        <v>9</v>
       </c>
       <c r="G10" t="s">
-        <v>89</v>
-      </c>
-      <c r="H10" t="s">
-        <v>87</v>
-      </c>
-      <c r="I10" t="s">
-        <v>86</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>70</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>38</v>
+        <v>71</v>
       </c>
       <c r="C11" s="2">
-        <v>0.05</v>
+        <v>14.9</v>
       </c>
       <c r="D11">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="E11" s="2">
         <f>$C11*$D11</f>
-        <v>0.45</v>
+        <v>14.9</v>
       </c>
       <c r="F11" t="s">
         <v>42</v>
       </c>
       <c r="G11" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
       <c r="H11" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
       <c r="I11" t="s">
-        <v>92</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="C12" s="2">
-        <v>0.1</v>
+        <v>3.73</v>
       </c>
       <c r="D12">
         <v>2</v>
       </c>
       <c r="E12" s="2">
         <f>$C12*$D12</f>
-        <v>0.2</v>
+        <v>7.46</v>
       </c>
       <c r="F12" t="s">
-        <v>42</v>
+        <v>9</v>
       </c>
       <c r="G12" t="s">
-        <v>99</v>
-      </c>
-      <c r="H12" t="s">
-        <v>87</v>
-      </c>
-      <c r="I12" t="s">
-        <v>100</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>41</v>
+        <v>14</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="C13" s="2">
-        <v>0.51</v>
+        <v>1.2</v>
       </c>
       <c r="D13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E13" s="2">
         <f>$C13*$D13</f>
-        <v>0.51</v>
+        <v>2.4</v>
       </c>
       <c r="F13" t="s">
-        <v>42</v>
+        <v>9</v>
       </c>
       <c r="G13" t="s">
-        <v>101</v>
-      </c>
-      <c r="H13" t="s">
-        <v>88</v>
-      </c>
-      <c r="I13" t="s">
-        <v>102</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>105</v>
+        <v>16</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="C14" s="2">
-        <v>0.28999999999999998</v>
+        <v>0.05</v>
       </c>
       <c r="D14">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E14" s="2">
         <f>$C14*$D14</f>
-        <v>1.7399999999999998</v>
+        <v>0.1</v>
       </c>
       <c r="F14" t="s">
-        <v>42</v>
+        <v>9</v>
       </c>
       <c r="G14" t="s">
-        <v>103</v>
-      </c>
-      <c r="H14" t="s">
-        <v>98</v>
-      </c>
-      <c r="I14" t="s">
-        <v>104</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>94</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="C15" s="2">
-        <v>2.16</v>
+        <v>5.98</v>
       </c>
       <c r="D15">
         <v>1</v>
       </c>
       <c r="E15" s="2">
         <f>$C15*$D15</f>
-        <v>2.16</v>
+        <v>5.98</v>
       </c>
       <c r="F15" t="s">
-        <v>42</v>
-      </c>
-      <c r="G15" t="s">
-        <v>95</v>
-      </c>
-      <c r="H15" t="s">
-        <v>96</v>
-      </c>
-      <c r="I15" t="s">
-        <v>97</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>27</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>50</v>
+        <v>76</v>
       </c>
       <c r="C16" s="2">
-        <v>16.899999999999999</v>
+        <v>1.82</v>
       </c>
       <c r="D16">
         <v>1</v>
       </c>
       <c r="E16" s="2">
         <f>$C16*$D16</f>
-        <v>16.899999999999999</v>
+        <v>1.82</v>
       </c>
       <c r="F16" t="s">
-        <v>42</v>
-      </c>
-      <c r="G16" t="s">
-        <v>53</v>
-      </c>
-      <c r="H16" t="s">
-        <v>52</v>
-      </c>
-      <c r="I16" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>47</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>55</v>
+        <v>77</v>
       </c>
       <c r="C17" s="2">
-        <v>1.64</v>
+        <v>1.82</v>
       </c>
       <c r="D17">
         <v>1</v>
       </c>
       <c r="E17" s="2">
         <f>$C17*$D17</f>
-        <v>1.64</v>
+        <v>1.82</v>
       </c>
       <c r="F17" t="s">
-        <v>42</v>
-      </c>
-      <c r="G17" t="s">
-        <v>56</v>
-      </c>
-      <c r="H17" t="s">
-        <v>43</v>
-      </c>
-      <c r="I17" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>68</v>
+        <v>22</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C18" s="2">
-        <v>1.25</v>
+        <v>0.1</v>
       </c>
       <c r="D18">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E18" s="2">
         <f>$C18*$D18</f>
-        <v>7.5</v>
+        <v>0.1</v>
       </c>
       <c r="F18" t="s">
-        <v>54</v>
-      </c>
-      <c r="G18" s="6">
-        <v>1559</v>
+        <v>42</v>
+      </c>
+      <c r="G18" t="s">
+        <v>89</v>
       </c>
       <c r="H18" t="s">
-        <v>54</v>
-      </c>
-      <c r="I18" s="6">
-        <v>1559</v>
+        <v>87</v>
+      </c>
+      <c r="I18" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="C19" s="2">
-        <v>0.59899999999999998</v>
+        <v>0.05</v>
       </c>
       <c r="D19">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E19" s="2">
         <f>$C19*$D19</f>
-        <v>0.59899999999999998</v>
+        <v>0.45</v>
       </c>
       <c r="F19" t="s">
-        <v>44</v>
+        <v>42</v>
+      </c>
+      <c r="G19" t="s">
+        <v>90</v>
+      </c>
+      <c r="H19" t="s">
+        <v>91</v>
+      </c>
+      <c r="I19" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>66</v>
+        <v>36</v>
       </c>
       <c r="C20" s="2">
-        <v>0.79</v>
+        <v>0.1</v>
       </c>
       <c r="D20">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="E20" s="2">
         <f>$C20*$D20</f>
-        <v>7.11</v>
+        <v>0.2</v>
       </c>
       <c r="F20" t="s">
-        <v>44</v>
+        <v>42</v>
+      </c>
+      <c r="G20" t="s">
+        <v>99</v>
+      </c>
+      <c r="H20" t="s">
+        <v>87</v>
+      </c>
+      <c r="I20" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>30</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>67</v>
+        <v>25</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="C21" s="2">
-        <v>0.99</v>
+        <v>0.51</v>
       </c>
       <c r="D21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E21" s="2">
         <f>$C21*$D21</f>
-        <v>1.98</v>
+        <v>0.51</v>
       </c>
       <c r="F21" t="s">
-        <v>44</v>
+        <v>42</v>
+      </c>
+      <c r="G21" t="s">
+        <v>101</v>
+      </c>
+      <c r="H21" t="s">
+        <v>88</v>
+      </c>
+      <c r="I21" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>26</v>
+        <v>105</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>69</v>
+        <v>40</v>
       </c>
       <c r="C22" s="2">
-        <v>0.09</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="D22">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E22" s="2">
         <f>$C22*$D22</f>
-        <v>0.27</v>
+        <v>1.7399999999999998</v>
       </c>
       <c r="F22" t="s">
-        <v>44</v>
+        <v>42</v>
+      </c>
+      <c r="G22" t="s">
+        <v>103</v>
+      </c>
+      <c r="H22" t="s">
+        <v>98</v>
+      </c>
+      <c r="I22" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>35</v>
+        <v>114</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>34</v>
+        <v>110</v>
       </c>
       <c r="C23" s="2">
-        <v>8.1000000000000003E-2</v>
+        <v>2.1</v>
       </c>
       <c r="D23">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E23" s="2">
         <f>$C23*$D23</f>
-        <v>0.56700000000000006</v>
+        <v>2.1</v>
       </c>
       <c r="F23" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="G23" t="s">
-        <v>62</v>
+        <v>111</v>
       </c>
       <c r="H23" t="s">
-        <v>61</v>
+        <v>112</v>
       </c>
       <c r="I23" t="s">
-        <v>63</v>
+        <v>113</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="C24" s="2">
-        <v>0.47</v>
+        <v>2.16</v>
       </c>
       <c r="D24">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E24" s="2">
         <f>$C24*$D24</f>
-        <v>1.88</v>
+        <v>2.16</v>
       </c>
       <c r="F24" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G24" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="H24" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
       <c r="I24" t="s">
-        <v>84</v>
+        <v>97</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>78</v>
+        <v>27</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="C25" s="2">
-        <v>5.98</v>
+        <v>16.899999999999999</v>
       </c>
       <c r="D25">
         <v>1</v>
       </c>
       <c r="E25" s="2">
         <f>$C25*$D25</f>
-        <v>5.98</v>
+        <v>16.899999999999999</v>
       </c>
       <c r="F25" t="s">
-        <v>49</v>
+        <v>42</v>
+      </c>
+      <c r="G25" t="s">
+        <v>53</v>
+      </c>
+      <c r="H25" t="s">
+        <v>52</v>
+      </c>
+      <c r="I25" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>76</v>
+        <v>47</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>55</v>
       </c>
       <c r="C26" s="2">
-        <v>1.82</v>
+        <v>1.64</v>
       </c>
       <c r="D26">
         <v>1</v>
       </c>
       <c r="E26" s="2">
         <f>$C26*$D26</f>
-        <v>1.82</v>
+        <v>1.64</v>
       </c>
       <c r="F26" t="s">
-        <v>49</v>
+        <v>42</v>
+      </c>
+      <c r="G26" t="s">
+        <v>56</v>
+      </c>
+      <c r="H26" t="s">
+        <v>43</v>
+      </c>
+      <c r="I26" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>77</v>
+        <v>68</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="C27" s="2">
-        <v>1.82</v>
+        <v>1.25</v>
       </c>
       <c r="D27">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E27" s="2">
         <f>$C27*$D27</f>
-        <v>1.82</v>
+        <v>7.5</v>
       </c>
       <c r="F27" t="s">
-        <v>49</v>
+        <v>54</v>
+      </c>
+      <c r="G27" s="6">
+        <v>1559</v>
+      </c>
+      <c r="H27" t="s">
+        <v>54</v>
+      </c>
+      <c r="I27" s="6">
+        <v>1559</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>79</v>
+        <v>28</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C28" s="2">
+        <v>0.59899999999999998</v>
       </c>
       <c r="D28">
         <v>1</v>
       </c>
+      <c r="E28" s="2">
+        <f>$C28*$D28</f>
+        <v>0.59899999999999998</v>
+      </c>
       <c r="F28" t="s">
-        <v>64</v>
+        <v>44</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>75</v>
+        <v>66</v>
+      </c>
+      <c r="C29" s="2">
+        <v>0.79</v>
       </c>
       <c r="D29">
-        <v>1</v>
+        <v>9</v>
+      </c>
+      <c r="E29" s="2">
+        <f>$C29*$D29</f>
+        <v>7.11</v>
       </c>
       <c r="F29" t="s">
-        <v>64</v>
+        <v>44</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>46</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>75</v>
+        <v>30</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C30" s="2">
+        <v>0.99</v>
       </c>
       <c r="D30">
         <v>2</v>
       </c>
+      <c r="E30" s="2">
+        <f>$C30*$D30</f>
+        <v>1.98</v>
+      </c>
       <c r="F30" t="s">
-        <v>64</v>
+        <v>44</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C31" s="2">
+        <v>0.09</v>
+      </c>
+      <c r="D31">
+        <v>3</v>
+      </c>
+      <c r="E31" s="2">
+        <f>$C31*$D31</f>
+        <v>0.27</v>
+      </c>
+      <c r="F31" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
         <v>48</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B32" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D31">
+      <c r="D32">
         <v>1</v>
       </c>
-      <c r="F31" t="s">
+      <c r="F32" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="38" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E38" s="5">
-        <f>SUM(E2:E37)</f>
-        <v>85.287999999999982</v>
+    <row r="35" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E35" s="5">
+        <f>SUM(E12:E32)</f>
+        <v>62.838999999999992</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" display="https://www.mcmaster.com/93465A113/" xr:uid="{30614124-8274-416D-BF4B-C61FC2A88B31}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{BC51F43F-73C3-4542-B883-85C971BB0C5E}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{6DDD143B-F9D0-4B29-A1DA-E8BD72E2D5ED}"/>
-    <hyperlink ref="B5" r:id="rId4" xr:uid="{C280DF8C-0D7D-4B6B-A819-A72B4DF674AB}"/>
-    <hyperlink ref="B7" r:id="rId5" xr:uid="{F7810F7C-7E96-4FB0-A9FF-0188B7A539E4}"/>
-    <hyperlink ref="B23" r:id="rId6" xr:uid="{A8CF3EA9-F882-4B3B-A679-5FBD485F406A}"/>
-    <hyperlink ref="B12" r:id="rId7" xr:uid="{D5B974E7-FB3C-41EF-B23E-71D65BA331EB}"/>
-    <hyperlink ref="B10" r:id="rId8" xr:uid="{2A361B31-C293-419F-8647-138083B24887}"/>
-    <hyperlink ref="B11" r:id="rId9" xr:uid="{F324FB64-F311-432C-85C3-C4A9CD2C260B}"/>
-    <hyperlink ref="B18" r:id="rId10" xr:uid="{46634537-F8C5-4322-89F5-5617EAA2C0B1}"/>
-    <hyperlink ref="B14" r:id="rId11" xr:uid="{D192A5CF-2E2F-48EE-B818-75B25482C472}"/>
-    <hyperlink ref="B13" r:id="rId12" xr:uid="{9B1C1D5D-2C03-47AA-BB33-8431974A2977}"/>
-    <hyperlink ref="B16" r:id="rId13" xr:uid="{EFBF539C-618E-43E0-A62F-575BF38DD6A9}"/>
-    <hyperlink ref="B17" r:id="rId14" xr:uid="{F1A68759-4C17-495E-AF4C-35EBB710BB0C}"/>
-    <hyperlink ref="B29" r:id="rId15" display="https://github.com/lafefspietz/MEMSduino/blob/main/3dprint_files/arduino-bracket.STL" xr:uid="{15E103AF-EAB5-4FDF-A5EE-5BBEEE5FC290}"/>
-    <hyperlink ref="B30" r:id="rId16" display="https://github.com/lafefspietz/MEMSduino/blob/main/3dprint_files/front-panel-edge-bracket.STL" xr:uid="{8CE89076-BF96-48E9-8823-7820AD88138C}"/>
-    <hyperlink ref="B19" r:id="rId17" xr:uid="{884619D7-502D-401A-901D-2363033DC363}"/>
-    <hyperlink ref="B31" r:id="rId18" xr:uid="{3ECC4416-4EC7-4521-89D4-53BB9BC8F581}"/>
-    <hyperlink ref="B20" r:id="rId19" xr:uid="{F448C947-6DA4-41EF-9F1C-DF0DACBB4455}"/>
-    <hyperlink ref="B21" r:id="rId20" display="https://www.amazon.com/ZYAMY-Dupont-Connector-Multicolor-Breadboard/dp/B0789F2Y1T/" xr:uid="{874914B1-8AFA-4BDC-8AC4-C9395C0DB705}"/>
-    <hyperlink ref="B9" r:id="rId21" xr:uid="{2C3ABC2D-CB2F-4186-90FB-491BEE516030}"/>
-    <hyperlink ref="B24" r:id="rId22" xr:uid="{8E0DEC65-6BCB-4630-B111-D454130D7E82}"/>
+    <hyperlink ref="B13" r:id="rId1" display="https://www.mcmaster.com/93465A113/" xr:uid="{30614124-8274-416D-BF4B-C61FC2A88B31}"/>
+    <hyperlink ref="B14" r:id="rId2" xr:uid="{6DDD143B-F9D0-4B29-A1DA-E8BD72E2D5ED}"/>
+    <hyperlink ref="B10" r:id="rId3" xr:uid="{C280DF8C-0D7D-4B6B-A819-A72B4DF674AB}"/>
+    <hyperlink ref="B3" r:id="rId4" xr:uid="{F7810F7C-7E96-4FB0-A9FF-0188B7A539E4}"/>
+    <hyperlink ref="B8" r:id="rId5" xr:uid="{A8CF3EA9-F882-4B3B-A679-5FBD485F406A}"/>
+    <hyperlink ref="B20" r:id="rId6" xr:uid="{D5B974E7-FB3C-41EF-B23E-71D65BA331EB}"/>
+    <hyperlink ref="B18" r:id="rId7" xr:uid="{2A361B31-C293-419F-8647-138083B24887}"/>
+    <hyperlink ref="B19" r:id="rId8" xr:uid="{F324FB64-F311-432C-85C3-C4A9CD2C260B}"/>
+    <hyperlink ref="B27" r:id="rId9" xr:uid="{46634537-F8C5-4322-89F5-5617EAA2C0B1}"/>
+    <hyperlink ref="B22" r:id="rId10" xr:uid="{D192A5CF-2E2F-48EE-B818-75B25482C472}"/>
+    <hyperlink ref="B21" r:id="rId11" xr:uid="{9B1C1D5D-2C03-47AA-BB33-8431974A2977}"/>
+    <hyperlink ref="B25" r:id="rId12" xr:uid="{EFBF539C-618E-43E0-A62F-575BF38DD6A9}"/>
+    <hyperlink ref="B26" r:id="rId13" xr:uid="{F1A68759-4C17-495E-AF4C-35EBB710BB0C}"/>
+    <hyperlink ref="B6" r:id="rId14" display="https://github.com/lafefspietz/MEMSduino/blob/main/3dprint_files/arduino-bracket.STL" xr:uid="{15E103AF-EAB5-4FDF-A5EE-5BBEEE5FC290}"/>
+    <hyperlink ref="B7" r:id="rId15" display="https://github.com/lafefspietz/MEMSduino/blob/main/3dprint_files/front-panel-edge-bracket.STL" xr:uid="{8CE89076-BF96-48E9-8823-7820AD88138C}"/>
+    <hyperlink ref="B28" r:id="rId16" xr:uid="{884619D7-502D-401A-901D-2363033DC363}"/>
+    <hyperlink ref="B32" r:id="rId17" xr:uid="{3ECC4416-4EC7-4521-89D4-53BB9BC8F581}"/>
+    <hyperlink ref="B29" r:id="rId18" xr:uid="{F448C947-6DA4-41EF-9F1C-DF0DACBB4455}"/>
+    <hyperlink ref="B30" r:id="rId19" display="https://www.amazon.com/ZYAMY-Dupont-Connector-Multicolor-Breadboard/dp/B0789F2Y1T/" xr:uid="{874914B1-8AFA-4BDC-8AC4-C9395C0DB705}"/>
+    <hyperlink ref="B11" r:id="rId20" xr:uid="{2C3ABC2D-CB2F-4186-90FB-491BEE516030}"/>
+    <hyperlink ref="B9" r:id="rId21" xr:uid="{8E0DEC65-6BCB-4630-B111-D454130D7E82}"/>
+    <hyperlink ref="B2" r:id="rId22" xr:uid="{7B560E24-64E6-4879-93DB-4D80FDE40F0B}"/>
+    <hyperlink ref="B12" r:id="rId23" xr:uid="{BC51F43F-73C3-4542-B883-85C971BB0C5E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId23"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId24"/>
 </worksheet>
 </file>
</xml_diff>